<commit_message>
Demo prep work - cleaned up gridScreen, graphExample, and selects.  Added grunt task for this demo.
</commit_message>
<xml_diff>
--- a/app/tables/graphExample/forms/graphExample/graphExample.xlsx
+++ b/app/tables/graphExample/forms/graphExample/graphExample.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="10500" windowWidth="31500" windowHeight="18900" activeTab="3"/>
+    <workbookView xWindow="4780" yWindow="5260" windowWidth="31500" windowHeight="18900"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
-    <sheet name="choices" sheetId="2" r:id="rId2"/>
-    <sheet name="queries" sheetId="3" r:id="rId3"/>
-    <sheet name="settings" sheetId="4" r:id="rId4"/>
+    <sheet name="queries" sheetId="3" r:id="rId2"/>
+    <sheet name="settings" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>comments</t>
   </si>
@@ -42,105 +41,12 @@
     <t>choice_filter</t>
   </si>
   <si>
-    <t>birds</t>
-  </si>
-  <si>
-    <t>blackbird</t>
-  </si>
-  <si>
-    <t>media/blackbird.png</t>
-  </si>
-  <si>
-    <t>bluethroat</t>
-  </si>
-  <si>
-    <t>media/bluethroat.png</t>
-  </si>
-  <si>
-    <t>crow</t>
-  </si>
-  <si>
-    <t>media/crow.png</t>
-  </si>
-  <si>
-    <t>eagle</t>
-  </si>
-  <si>
-    <t>media/eagle.png</t>
-  </si>
-  <si>
-    <t>egret</t>
-  </si>
-  <si>
-    <t>media/egret.png</t>
-  </si>
-  <si>
-    <t>gull</t>
-  </si>
-  <si>
-    <t>media/gull.png</t>
-  </si>
-  <si>
-    <t>hawfinch</t>
-  </si>
-  <si>
-    <t>media/hawfinch.png</t>
-  </si>
-  <si>
-    <t>yes_no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>colors</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
     <t>uri</t>
   </si>
   <si>
     <t>callback</t>
   </si>
   <si>
-    <t>countries</t>
-  </si>
-  <si>
-    <t>"https://query.yahooapis.com/v1/public/yql?format=json&amp;q=" +  encodeURIComponent("select * from geo.countries where place='North America'")</t>
-  </si>
-  <si>
-    <t>states</t>
-  </si>
-  <si>
-    <t>"https://query.yahooapis.com/v1/public/yql?format=json&amp;q=" +  encodeURIComponent("select * from geo.states where place='" + data('country') + "'")</t>
-  </si>
-  <si>
     <t>regions_csv</t>
   </si>
   <si>
@@ -171,15 +77,6 @@
     <t>query_name</t>
   </si>
   <si>
-    <t>choice_list_name</t>
-  </si>
-  <si>
-    <t>data_value</t>
-  </si>
-  <si>
-    <t>display.image</t>
-  </si>
-  <si>
     <t>display.text</t>
   </si>
   <si>
@@ -193,14 +90,6 @@
   </si>
   <si>
     <t>hideInContents</t>
-  </si>
-  <si>
-    <t>context.query.results ? _.map(context.query.results.place, function(place){
-place.label = place.name;
-place.data_value = place.name;
-place.display = {text:place.label};
-return place;
-}) : []</t>
   </si>
   <si>
     <t>_.chain(context).pluck('region').uniq().map(function(region){
@@ -217,96 +106,18 @@
 })</t>
   </si>
   <si>
-    <t>holidays</t>
-  </si>
-  <si>
-    <t>foods</t>
-  </si>
-  <si>
-    <t>Milk</t>
-  </si>
-  <si>
-    <t>Bread</t>
-  </si>
-  <si>
-    <t>Fruit</t>
-  </si>
-  <si>
-    <t>Meat</t>
-  </si>
-  <si>
-    <t>Vegetable</t>
-  </si>
-  <si>
-    <t>milk</t>
-  </si>
-  <si>
-    <t>bread</t>
-  </si>
-  <si>
-    <t>meat</t>
-  </si>
-  <si>
-    <t>fruit</t>
-  </si>
-  <si>
-    <t>vegetable</t>
-  </si>
-  <si>
-    <t>christmas</t>
-  </si>
-  <si>
-    <t>Christmas</t>
-  </si>
-  <si>
     <t>query_type</t>
   </si>
   <si>
-    <t>ajax</t>
-  </si>
-  <si>
     <t>csv</t>
   </si>
   <si>
-    <t>kwanzaa</t>
-  </si>
-  <si>
-    <t>Kwanzaa</t>
-  </si>
-  <si>
-    <t>hannukah</t>
-  </si>
-  <si>
-    <t>Hannukah</t>
-  </si>
-  <si>
-    <t>Diwali</t>
-  </si>
-  <si>
-    <t>diwali</t>
-  </si>
-  <si>
-    <t>media/kingfisher.png</t>
-  </si>
-  <si>
-    <t>media/robin.png</t>
-  </si>
-  <si>
-    <t>kingfisher</t>
-  </si>
-  <si>
-    <t>robin</t>
-  </si>
-  <si>
     <t>display.audio</t>
   </si>
   <si>
     <t>display.video</t>
   </si>
   <si>
-    <t>sexes</t>
-  </si>
-  <si>
     <t>constraint</t>
   </si>
   <si>
@@ -314,24 +125,6 @@
   </si>
   <si>
     <t>templatePath</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>grey</t>
-  </si>
-  <si>
-    <t>Grey</t>
-  </si>
-  <si>
-    <t>brown</t>
-  </si>
-  <si>
-    <t>White</t>
   </si>
   <si>
     <t>graphExample</t>
@@ -1056,7 +849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -1078,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1087,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1096,75 +889,75 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="L1" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="M1" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="12.75" customHeight="1">
       <c r="D2" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>115</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="12.75" customHeight="1">
       <c r="D3" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="12.75" customHeight="1">
       <c r="D4" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="12.75" customHeight="1">
       <c r="D5" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="17.5" customHeight="1">
@@ -1187,329 +980,115 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="1" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="87.33203125" customWidth="1"/>
+    <col min="4" max="4" width="76.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.75" customHeight="1">
+    <row r="1" spans="1:4" ht="34.5" customHeight="1">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.75" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34.5" customHeight="1">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.75" customHeight="1">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34.5" customHeight="1">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.75" customHeight="1">
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.25" customHeight="1">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.75" customHeight="1">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.25" customHeight="1">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16.75" customHeight="1">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.25" customHeight="1">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16.75" customHeight="1">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.25" customHeight="1">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16.75" customHeight="1">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16.75" customHeight="1">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.75" customHeight="1">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16.75" customHeight="1"/>
-    <row r="12" spans="1:4" ht="16.75" customHeight="1">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16.75" customHeight="1">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16.75" customHeight="1"/>
-    <row r="15" spans="1:4" ht="16.75" customHeight="1">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16.75" customHeight="1">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16.75" customHeight="1">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16.75" customHeight="1">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16.75" customHeight="1">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16.75" customHeight="1"/>
-    <row r="21" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A32" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A33" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" t="s">
-        <v>94</v>
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1525,161 +1104,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="87.33203125" customWidth="1"/>
-    <col min="4" max="4" width="76.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="34.5" customHeight="1">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="34.5" customHeight="1">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="34.5" customHeight="1">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="34.5" customHeight="1">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="34.5" customHeight="1">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1690,27 +1117,27 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="16.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>20130408</v>
@@ -1718,15 +1145,15 @@
     </row>
     <row r="4" spans="1:3" ht="16.75" customHeight="1">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.75" customHeight="1">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>

</xml_diff>